<commit_message>
Allow for multiple template documents for secondaries
</commit_message>
<xml_diff>
--- a/public/sample_uploads/offers.xlsx
+++ b/public/sample_uploads/offers.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A0A44D6-F95B-4DE1-B035-ADBC3F1B3425}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63FADA69-1E2D-4B38-B402-584B7D26C445}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,13 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
-  <si>
-    <t>Quantity</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
   <si>
     <t>Address</t>
   </si>
@@ -98,6 +92,45 @@
   </si>
   <si>
     <t>emp4@myfirm.com</t>
+  </si>
+  <si>
+    <t>Middle Name</t>
+  </si>
+  <si>
+    <t>Emp1</t>
+  </si>
+  <si>
+    <t>Emp2</t>
+  </si>
+  <si>
+    <t>Emp3</t>
+  </si>
+  <si>
+    <t>Emp4</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>James</t>
+  </si>
+  <si>
+    <t>Jim</t>
+  </si>
+  <si>
+    <t>Jack</t>
+  </si>
+  <si>
+    <t>First Name *</t>
+  </si>
+  <si>
+    <t>User (email) *</t>
+  </si>
+  <si>
+    <t>Offer Quantity *</t>
+  </si>
+  <si>
+    <t>Last Name *</t>
   </si>
 </sst>
 </file>
@@ -152,10 +185,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -472,158 +506,201 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" showOutlineSymbols="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" showOutlineSymbols="0" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.46484375" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13.265625" customWidth="1"/>
-    <col min="2" max="2" width="28.9296875" customWidth="1"/>
-    <col min="3" max="3" width="84.46484375" customWidth="1"/>
-    <col min="4" max="4" width="15.6640625" customWidth="1"/>
-    <col min="5" max="5" width="18.06640625" customWidth="1"/>
-    <col min="6" max="6" width="16.86328125" customWidth="1"/>
-    <col min="1011" max="1024" width="11.53125" customWidth="1"/>
+    <col min="2" max="5" width="28.9296875" customWidth="1"/>
+    <col min="6" max="6" width="84.46484375" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" customWidth="1"/>
+    <col min="8" max="8" width="18.06640625" customWidth="1"/>
+    <col min="9" max="9" width="16.86328125" customWidth="1"/>
+    <col min="1014" max="1027" width="11.53125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="J1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="K1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
     </row>
-    <row r="2" spans="1:8" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>10</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="1">
+        <v>3786205303</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="J2">
+        <v>111111</v>
+      </c>
+      <c r="K2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="1">
-        <v>3786205303</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2">
-        <v>111111</v>
-      </c>
-      <c r="H2" t="s">
-        <v>11</v>
-      </c>
     </row>
-    <row r="3" spans="1:8" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>20</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="1">
+        <v>7381987473</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="1">
-        <v>7381987473</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3">
+      <c r="J3">
         <v>222222</v>
       </c>
-      <c r="H3" t="s">
-        <v>11</v>
+      <c r="K3" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>30</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="1">
+        <v>4930128680</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="J4">
+        <v>333333</v>
+      </c>
+      <c r="K4" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="1">
-        <v>4930128680</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4">
-        <v>333333</v>
-      </c>
-      <c r="H4" t="s">
-        <v>18</v>
-      </c>
     </row>
-    <row r="5" spans="1:8" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>40</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="1">
+        <v>2962756900</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="1">
-        <v>2962756900</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5">
+      <c r="J5">
         <v>444444</v>
       </c>
-      <c r="H5" t="s">
-        <v>18</v>
+      <c r="K5" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" ht="13.5" x14ac:dyDescent="0.35">
       <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:8" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" ht="13.5" x14ac:dyDescent="0.35">
       <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
Removed unwanted cols from offer import
</commit_message>
<xml_diff>
--- a/public/sample_uploads/offers.xlsx
+++ b/public/sample_uploads/offers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B72B269-B527-488E-9CB6-097514DFB772}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05E79CF0-4905-481C-BF99-7E679D617119}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
   <si>
     <t>Address</t>
   </si>
@@ -89,9 +89,6 @@
   </si>
   <si>
     <t>emp4@myfirm.com</t>
-  </si>
-  <si>
-    <t>Middle Name</t>
   </si>
   <si>
     <t>Emp1</t>
@@ -505,57 +502,56 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" showOutlineSymbols="0" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" showOutlineSymbols="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.46484375" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13.265625" customWidth="1"/>
-    <col min="2" max="5" width="28.9296875" customWidth="1"/>
-    <col min="6" max="6" width="84.46484375" customWidth="1"/>
-    <col min="7" max="7" width="15.6640625" customWidth="1"/>
-    <col min="8" max="8" width="18.06640625" customWidth="1"/>
-    <col min="9" max="9" width="16.86328125" customWidth="1"/>
-    <col min="1014" max="1027" width="11.53125" customWidth="1"/>
+    <col min="2" max="4" width="28.9296875" customWidth="1"/>
+    <col min="5" max="5" width="84.46484375" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" customWidth="1"/>
+    <col min="7" max="7" width="18.06640625" customWidth="1"/>
+    <col min="8" max="8" width="16.86328125" customWidth="1"/>
+    <col min="1013" max="1026" width="11.53125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="I1" t="s">
+        <v>3</v>
+      </c>
       <c r="J1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>10</v>
       </c>
@@ -563,32 +559,31 @@
         <v>19</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2" t="s">
-        <v>28</v>
+        <v>23</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="1">
+      <c r="G2" s="1">
         <v>3786205303</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J2">
+      <c r="I2">
         <v>111111</v>
       </c>
-      <c r="K2" t="s">
+      <c r="J2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>20</v>
       </c>
@@ -596,32 +591,31 @@
         <v>20</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="1">
+      <c r="G3" s="1">
         <v>7381987473</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J3">
+      <c r="I3">
         <v>222222</v>
       </c>
-      <c r="K3" t="s">
+      <c r="J3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>30</v>
       </c>
@@ -629,32 +623,31 @@
         <v>21</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="1">
+      <c r="G4" s="1">
         <v>4930128680</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="J4">
+      <c r="I4">
         <v>333333</v>
       </c>
-      <c r="K4" t="s">
+      <c r="J4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>40</v>
       </c>
@@ -662,42 +655,39 @@
         <v>22</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="1">
+      <c r="G5" s="1">
         <v>2962756900</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J5">
+      <c r="I5">
         <v>444444</v>
       </c>
-      <c r="K5" t="s">
+      <c r="J5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="13.5" x14ac:dyDescent="0.35">
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:11" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" ht="13.5" x14ac:dyDescent="0.35">
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
Offer import now support investor offers
</commit_message>
<xml_diff>
--- a/public/sample_uploads/offers.xlsx
+++ b/public/sample_uploads/offers.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05E79CF0-4905-481C-BF99-7E679D617119}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFDADC33-DA5D-44AE-BDB9-203F16C2F814}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
   <si>
     <t>Address</t>
   </si>
@@ -128,13 +128,25 @@
   </si>
   <si>
     <t>Bank Account</t>
+  </si>
+  <si>
+    <t>Founder</t>
+  </si>
+  <si>
+    <t>Employee</t>
+  </si>
+  <si>
+    <t>Founder/Employee/Investor *</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Investor </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -159,6 +171,13 @@
       <family val="1"/>
       <charset val="1"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -177,17 +196,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
     <cellStyle name="Normal 3" xfId="2" xr:uid="{E1D866A5-6C15-4F3C-952F-A61DF9E19082}"/>
@@ -502,194 +524,220 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.46484375" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13.265625" customWidth="1"/>
-    <col min="2" max="4" width="28.9296875" customWidth="1"/>
-    <col min="5" max="5" width="84.46484375" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" customWidth="1"/>
-    <col min="7" max="7" width="18.06640625" customWidth="1"/>
-    <col min="8" max="8" width="16.86328125" customWidth="1"/>
-    <col min="1013" max="1026" width="11.53125" customWidth="1"/>
+    <col min="2" max="3" width="28.3984375" customWidth="1"/>
+    <col min="4" max="6" width="28.9296875" customWidth="1"/>
+    <col min="7" max="7" width="84.46484375" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" customWidth="1"/>
+    <col min="9" max="9" width="18.06640625" customWidth="1"/>
+    <col min="10" max="10" width="16.86328125" customWidth="1"/>
+    <col min="1015" max="1028" width="11.53125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>3</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>10</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="1">
+      <c r="I2" s="1">
         <v>3786205303</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I2">
+      <c r="K2">
         <v>111111</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>20</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="1">
+      <c r="I3" s="1">
         <v>7381987473</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I3">
+      <c r="K3">
         <v>222222</v>
       </c>
-      <c r="J3" t="s">
+      <c r="L3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>30</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="1">
+      <c r="I4" s="1">
         <v>4930128680</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I4">
+      <c r="K4">
         <v>333333</v>
       </c>
-      <c r="J4" t="s">
+      <c r="L4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>40</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="1">
+      <c r="I5" s="1">
         <v>2962756900</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I5">
+      <c r="K5">
         <v>444444</v>
       </c>
-      <c r="J5" t="s">
+      <c r="L5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
+    <row r="6" spans="1:12" ht="13.5" x14ac:dyDescent="0.35">
       <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
     </row>
-    <row r="7" spans="1:10" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
+    <row r="7" spans="1:12" ht="13.5" x14ac:dyDescent="0.35">
       <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D4" r:id="rId1" xr:uid="{19704892-9206-47E5-A980-C3922B32D904}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>

</xml_diff>

<commit_message>
Added update only to offer import
</commit_message>
<xml_diff>
--- a/public/sample_uploads/offers.xlsx
+++ b/public/sample_uploads/offers.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{080B46F7-CC2D-4121-9A54-D799A4C8741F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59B9270D-74A3-4559-8D42-1978133A95EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="55">
   <si>
     <t>Address</t>
   </si>
@@ -179,6 +179,12 @@
   </si>
   <si>
     <t>Investor 2</t>
+  </si>
+  <si>
+    <t>Update Only</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -564,10 +570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView tabSelected="1" showOutlineSymbols="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" showOutlineSymbols="0" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3:M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.46484375" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -582,7 +588,7 @@
     <col min="1015" max="1028" width="11.53125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
@@ -619,8 +625,11 @@
       <c r="L1" t="s">
         <v>4</v>
       </c>
+      <c r="M1" s="4" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>10</v>
       </c>
@@ -655,8 +664,11 @@
       <c r="L2" t="s">
         <v>8</v>
       </c>
+      <c r="M2" s="4" t="s">
+        <v>54</v>
+      </c>
     </row>
-    <row r="3" spans="1:12" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>20</v>
       </c>
@@ -691,8 +703,11 @@
       <c r="L3" t="s">
         <v>8</v>
       </c>
+      <c r="M3" s="4" t="s">
+        <v>54</v>
+      </c>
     </row>
-    <row r="4" spans="1:12" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>30</v>
       </c>
@@ -727,8 +742,11 @@
       <c r="L4" t="s">
         <v>15</v>
       </c>
+      <c r="M4" s="4" t="s">
+        <v>54</v>
+      </c>
     </row>
-    <row r="5" spans="1:12" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>40</v>
       </c>
@@ -763,12 +781,15 @@
       <c r="L5" t="s">
         <v>15</v>
       </c>
+      <c r="M5" s="4" t="s">
+        <v>54</v>
+      </c>
     </row>
-    <row r="6" spans="1:12" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="4">
+    <row r="6" spans="1:13" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="1">
         <v>10</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="1" t="s">
         <v>40</v>
       </c>
       <c r="C6" t="s">
@@ -789,24 +810,27 @@
       <c r="H6" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6" s="1">
         <v>209989880</v>
       </c>
-      <c r="J6" s="4" t="s">
+      <c r="J6" s="1" t="s">
         <v>45</v>
       </c>
       <c r="K6">
         <v>5555</v>
       </c>
-      <c r="L6" s="4" t="s">
+      <c r="L6" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="M6" s="4" t="s">
+        <v>54</v>
+      </c>
     </row>
-    <row r="7" spans="1:12" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="4">
+    <row r="7" spans="1:13" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="1">
         <v>10</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="1" t="s">
         <v>40</v>
       </c>
       <c r="C7" t="s">
@@ -827,17 +851,20 @@
       <c r="H7" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I7" s="1">
         <v>8273487234</v>
       </c>
-      <c r="J7" s="4" t="s">
+      <c r="J7" s="1" t="s">
         <v>50</v>
       </c>
       <c r="K7">
         <v>6666</v>
       </c>
-      <c r="L7" s="4" t="s">
+      <c r="L7" s="1" t="s">
         <v>15</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fiexd offer completion report
</commit_message>
<xml_diff>
--- a/public/sample_uploads/offers.xlsx
+++ b/public/sample_uploads/offers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59B9270D-74A3-4559-8D42-1978133A95EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10F2762A-0634-4D87-B435-A783FE04EEF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,14 +20,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="57">
   <si>
     <t>Address</t>
   </si>
   <si>
-    <t>PAN</t>
-  </si>
-  <si>
     <t>IFSC Code</t>
   </si>
   <si>
@@ -185,6 +182,15 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>Pan</t>
+  </si>
+  <si>
+    <t>DP</t>
+  </si>
+  <si>
+    <t>Client Id</t>
   </si>
 </sst>
 </file>
@@ -570,10 +576,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView tabSelected="1" showOutlineSymbols="0" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3:M7"/>
+    <sheetView tabSelected="1" showOutlineSymbols="0" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.46484375" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -588,283 +594,325 @@
     <col min="1015" max="1028" width="11.53125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>33</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" t="s">
         <v>2</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>3</v>
       </c>
-      <c r="L1" t="s">
-        <v>4</v>
-      </c>
       <c r="M1" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>6</v>
       </c>
       <c r="I2" s="1">
         <v>3786205303</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K2">
         <v>111111</v>
       </c>
       <c r="L2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
+      </c>
+      <c r="N2">
+        <v>123456</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>20</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="I3" s="1">
         <v>7381987473</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K3">
         <v>222222</v>
       </c>
       <c r="L3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
+      </c>
+      <c r="N3">
+        <v>234567</v>
+      </c>
+      <c r="O3">
+        <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>30</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="I4" s="1">
         <v>4930128680</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K4">
         <v>333333</v>
       </c>
       <c r="L4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
+      </c>
+      <c r="N4">
+        <v>345678</v>
+      </c>
+      <c r="O4">
+        <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>40</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="I5" s="1">
         <v>2962756900</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K5">
         <v>444444</v>
       </c>
       <c r="L5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
+      </c>
+      <c r="N5">
+        <v>456789</v>
+      </c>
+      <c r="O5">
+        <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C6" t="s">
-        <v>51</v>
-      </c>
-      <c r="D6" s="3" t="s">
+      <c r="G6" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="G6" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>44</v>
       </c>
       <c r="I6" s="1">
         <v>209989880</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K6">
         <v>5555</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
+      </c>
+      <c r="N6">
+        <v>567900</v>
+      </c>
+      <c r="O6">
+        <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>10</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D7" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="G7" s="1" t="s">
+      <c r="H7" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>49</v>
       </c>
       <c r="I7" s="1">
         <v>8273487234</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K7">
         <v>6666</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
+      </c>
+      <c r="N7">
+        <v>679011</v>
+      </c>
+      <c r="O7">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sale fixes 1 (#324)
* Better message for Accept SPA email

* Allow support to edit and view sale

* SkipNotification is broken

* Added ransack for holdings

* Show investors offers on dashboard, for only active sales

* Changed steps for offer card

* Allocation job now gives realtime updates on progress

* Fixed rubocop errors

* Added offer_steps

* Added offer_steps
</commit_message>
<xml_diff>
--- a/public/sample_uploads/offers.xlsx
+++ b/public/sample_uploads/offers.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10F2762A-0634-4D87-B435-A783FE04EEF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81F30578-8B71-4E8F-A22E-444BE0132A14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="58">
   <si>
     <t>Address</t>
   </si>
@@ -191,6 +191,9 @@
   </si>
   <si>
     <t>Client Id</t>
+  </si>
+  <si>
+    <t>Seller Signatory Emails</t>
   </si>
 </sst>
 </file>
@@ -253,12 +256,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
@@ -576,10 +578,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:P7"/>
   <sheetViews>
-    <sheetView tabSelected="1" showOutlineSymbols="0" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+    <sheetView tabSelected="1" showOutlineSymbols="0" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.46484375" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -588,13 +590,13 @@
     <col min="2" max="3" width="28.3984375" customWidth="1"/>
     <col min="4" max="6" width="28.9296875" customWidth="1"/>
     <col min="7" max="7" width="84.46484375" customWidth="1"/>
-    <col min="8" max="8" width="15.6640625" customWidth="1"/>
-    <col min="9" max="9" width="18.06640625" customWidth="1"/>
-    <col min="10" max="10" width="16.86328125" customWidth="1"/>
-    <col min="1015" max="1028" width="11.53125" customWidth="1"/>
+    <col min="8" max="9" width="15.6640625" customWidth="1"/>
+    <col min="10" max="10" width="18.06640625" customWidth="1"/>
+    <col min="11" max="11" width="16.86328125" customWidth="1"/>
+    <col min="1016" max="1029" width="11.53125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>31</v>
       </c>
@@ -620,28 +622,31 @@
         <v>54</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>2</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>3</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="O1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="P1" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>10</v>
       </c>
@@ -664,29 +669,32 @@
       <c r="H2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="1">
+      <c r="I2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="1">
         <v>3786205303</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>111111</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>7</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="N2" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>123456</v>
       </c>
-      <c r="O2">
+      <c r="P2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>20</v>
       </c>
@@ -709,29 +717,32 @@
       <c r="H3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="1">
+      <c r="I3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="1">
         <v>7381987473</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>222222</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>7</v>
       </c>
-      <c r="M3" s="4" t="s">
+      <c r="N3" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>234567</v>
       </c>
-      <c r="O3">
+      <c r="P3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>30</v>
       </c>
@@ -754,29 +765,32 @@
       <c r="H4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I4" s="1">
+      <c r="I4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4" s="1">
         <v>4930128680</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>333333</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>14</v>
       </c>
-      <c r="M4" s="4" t="s">
+      <c r="N4" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="N4">
+      <c r="O4">
         <v>345678</v>
       </c>
-      <c r="O4">
+      <c r="P4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>40</v>
       </c>
@@ -799,29 +813,32 @@
       <c r="H5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I5" s="1">
+      <c r="I5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J5" s="1">
         <v>2962756900</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="K5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>444444</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>14</v>
       </c>
-      <c r="M5" s="4" t="s">
+      <c r="N5" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="N5">
+      <c r="O5">
         <v>456789</v>
       </c>
-      <c r="O5">
+      <c r="P5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>10</v>
       </c>
@@ -846,29 +863,32 @@
       <c r="H6" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="I6" s="1">
+      <c r="I6" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="J6" s="1">
         <v>209989880</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="K6" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>5555</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="M6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="M6" s="4" t="s">
+      <c r="N6" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="N6">
+      <c r="O6">
         <v>567900</v>
       </c>
-      <c r="O6">
+      <c r="P6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>10</v>
       </c>
@@ -893,25 +913,28 @@
       <c r="H7" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="I7" s="1">
+      <c r="I7" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="J7" s="1">
         <v>8273487234</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="K7" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <v>6666</v>
       </c>
-      <c r="L7" s="1" t="s">
+      <c r="M7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="M7" s="4" t="s">
+      <c r="N7" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="N7">
+      <c r="O7">
         <v>679011</v>
       </c>
-      <c r="O7">
+      <c r="P7">
         <v>6</v>
       </c>
     </row>
@@ -920,6 +943,9 @@
     <hyperlink ref="D4" r:id="rId1" xr:uid="{19704892-9206-47E5-A980-C3922B32D904}"/>
     <hyperlink ref="D6" r:id="rId2" xr:uid="{C08A49CB-44D2-4524-A8CA-AC4C24AEC5DC}"/>
     <hyperlink ref="D7" r:id="rId3" xr:uid="{A926393F-6D22-4C7F-AFD9-06DF376D31F7}"/>
+    <hyperlink ref="I4" r:id="rId4" xr:uid="{C84373C9-1565-4B62-96B2-218A347D68E8}"/>
+    <hyperlink ref="I6" r:id="rId5" xr:uid="{3032ED9C-BF7B-4835-B707-8EBF94637F00}"/>
+    <hyperlink ref="I7" r:id="rId6" xr:uid="{82419342-953D-4B49-93FF-7C924BB80AC1}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Fixed import of offers and interests, directly from downloads
</commit_message>
<xml_diff>
--- a/public/sample_uploads/offers.xlsx
+++ b/public/sample_uploads/offers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F84160AE-0A53-4B53-BDCA-61E37F709BB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{826C0D56-EEFE-4D04-BA0E-FA0E04D11AEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15" yWindow="735" windowWidth="23985" windowHeight="14265" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="55">
   <si>
     <t>Address</t>
   </si>
@@ -88,39 +88,6 @@
     <t>emp4@myfirm.com</t>
   </si>
   <si>
-    <t>Emp1</t>
-  </si>
-  <si>
-    <t>Emp2</t>
-  </si>
-  <si>
-    <t>Emp3</t>
-  </si>
-  <si>
-    <t>Emp4</t>
-  </si>
-  <si>
-    <t>John</t>
-  </si>
-  <si>
-    <t>James</t>
-  </si>
-  <si>
-    <t>Jim</t>
-  </si>
-  <si>
-    <t>Jack</t>
-  </si>
-  <si>
-    <t>First Name *</t>
-  </si>
-  <si>
-    <t>Offer Quantity *</t>
-  </si>
-  <si>
-    <t>Last Name *</t>
-  </si>
-  <si>
     <t>Email *</t>
   </si>
   <si>
@@ -142,9 +109,6 @@
     <t>Investor</t>
   </si>
   <si>
-    <t>Investor1</t>
-  </si>
-  <si>
     <t>emp1@investor1.com</t>
   </si>
   <si>
@@ -157,9 +121,6 @@
     <t>AX1123MM</t>
   </si>
   <si>
-    <t>Investor2</t>
-  </si>
-  <si>
     <t>emp1@investor2.com</t>
   </si>
   <si>
@@ -200,6 +161,30 @@
   </si>
   <si>
     <t>Approved*</t>
+  </si>
+  <si>
+    <t>Quantity *</t>
+  </si>
+  <si>
+    <t>Full Name *</t>
+  </si>
+  <si>
+    <t>Emp1 John</t>
+  </si>
+  <si>
+    <t>Emp2 James</t>
+  </si>
+  <si>
+    <t>Emp3 Jim</t>
+  </si>
+  <si>
+    <t>Emp4 Jack</t>
+  </si>
+  <si>
+    <t>Emp1 Investor1</t>
+  </si>
+  <si>
+    <t>Emp1 Investor2</t>
   </si>
 </sst>
 </file>
@@ -584,81 +569,78 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R7"/>
+  <dimension ref="A1:Q7"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="G1" sqref="G1:G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.46484375" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="3" width="13.265625" customWidth="1"/>
     <col min="4" max="5" width="28.3984375" customWidth="1"/>
-    <col min="6" max="8" width="28.9296875" customWidth="1"/>
-    <col min="9" max="9" width="84.46484375" customWidth="1"/>
-    <col min="10" max="11" width="15.6640625" customWidth="1"/>
-    <col min="12" max="12" width="18.06640625" customWidth="1"/>
-    <col min="13" max="13" width="16.86328125" customWidth="1"/>
-    <col min="1018" max="1031" width="11.53125" customWidth="1"/>
+    <col min="6" max="7" width="28.9296875" customWidth="1"/>
+    <col min="8" max="8" width="84.46484375" customWidth="1"/>
+    <col min="9" max="10" width="15.6640625" customWidth="1"/>
+    <col min="11" max="11" width="18.06640625" customWidth="1"/>
+    <col min="12" max="12" width="16.86328125" customWidth="1"/>
+    <col min="1017" max="1030" width="11.53125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>56</v>
+        <v>23</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="M1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="M1" t="s">
+        <v>2</v>
+      </c>
       <c r="N1" t="s">
-        <v>2</v>
-      </c>
-      <c r="O1" t="s">
         <v>3</v>
       </c>
+      <c r="O1" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="P1" s="1" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>10</v>
       </c>
@@ -666,53 +648,50 @@
         <v>100</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="2" t="s">
         <v>18</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>26</v>
+        <v>49</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="L2" s="1">
+      <c r="K2" s="1">
         <v>3786205303</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="N2">
+      <c r="M2">
         <v>111111</v>
       </c>
-      <c r="O2" t="s">
+      <c r="N2" t="s">
         <v>7</v>
       </c>
-      <c r="P2" s="1" t="s">
-        <v>53</v>
+      <c r="O2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P2">
+        <v>123456</v>
       </c>
       <c r="Q2">
-        <v>123456</v>
-      </c>
-      <c r="R2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>20</v>
       </c>
@@ -720,53 +699,50 @@
         <v>100</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="2" t="s">
         <v>19</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>27</v>
+        <v>50</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="L3" s="1">
+      <c r="K3" s="1">
         <v>7381987473</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="N3">
+      <c r="M3">
         <v>222222</v>
       </c>
-      <c r="O3" t="s">
+      <c r="N3" t="s">
         <v>7</v>
       </c>
-      <c r="P3" s="1" t="s">
-        <v>53</v>
+      <c r="O3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P3">
+        <v>234567</v>
       </c>
       <c r="Q3">
-        <v>234567</v>
-      </c>
-      <c r="R3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>30</v>
       </c>
@@ -774,53 +750,50 @@
         <v>100</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="3" t="s">
         <v>20</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>28</v>
+        <v>51</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="J4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="L4" s="1">
+      <c r="K4" s="1">
         <v>4930128680</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="L4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="N4">
+      <c r="M4">
         <v>333333</v>
       </c>
-      <c r="O4" t="s">
+      <c r="N4" t="s">
         <v>14</v>
       </c>
-      <c r="P4" s="1" t="s">
-        <v>53</v>
+      <c r="O4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P4">
+        <v>345678</v>
       </c>
       <c r="Q4">
-        <v>345678</v>
-      </c>
-      <c r="R4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>40</v>
       </c>
@@ -828,53 +801,50 @@
         <v>100</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="2" t="s">
         <v>21</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>29</v>
+        <v>52</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="J5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="L5" s="1">
+      <c r="K5" s="1">
         <v>2962756900</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="L5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="N5">
+      <c r="M5">
         <v>444444</v>
       </c>
-      <c r="O5" t="s">
+      <c r="N5" t="s">
         <v>14</v>
       </c>
-      <c r="P5" s="1" t="s">
-        <v>53</v>
+      <c r="O5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P5">
+        <v>456789</v>
       </c>
       <c r="Q5">
-        <v>456789</v>
-      </c>
-      <c r="R5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>10</v>
       </c>
@@ -882,55 +852,52 @@
         <v>100</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E6" t="s">
-        <v>50</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>40</v>
+      <c r="H6" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="L6" s="1">
+        <v>31</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K6" s="1">
         <v>209989880</v>
       </c>
-      <c r="M6" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="N6">
+      <c r="L6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M6">
         <v>5555</v>
       </c>
+      <c r="N6" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="O6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>53</v>
+        <v>40</v>
+      </c>
+      <c r="P6">
+        <v>567900</v>
       </c>
       <c r="Q6">
-        <v>567900</v>
-      </c>
-      <c r="R6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>10</v>
       </c>
@@ -938,51 +905,48 @@
         <v>100</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="E7" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>45</v>
+        <v>54</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="L7" s="1">
+        <v>35</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K7" s="1">
         <v>8273487234</v>
       </c>
-      <c r="M7" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="N7">
+      <c r="L7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M7">
         <v>6666</v>
       </c>
+      <c r="N7" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="O7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P7" s="1" t="s">
-        <v>53</v>
+        <v>40</v>
+      </c>
+      <c r="P7">
+        <v>679011</v>
       </c>
       <c r="Q7">
-        <v>679011</v>
-      </c>
-      <c r="R7">
         <v>6</v>
       </c>
     </row>
@@ -991,9 +955,9 @@
     <hyperlink ref="F4" r:id="rId1" xr:uid="{19704892-9206-47E5-A980-C3922B32D904}"/>
     <hyperlink ref="F6" r:id="rId2" xr:uid="{C08A49CB-44D2-4524-A8CA-AC4C24AEC5DC}"/>
     <hyperlink ref="F7" r:id="rId3" xr:uid="{A926393F-6D22-4C7F-AFD9-06DF376D31F7}"/>
-    <hyperlink ref="K4" r:id="rId4" xr:uid="{C84373C9-1565-4B62-96B2-218A347D68E8}"/>
-    <hyperlink ref="K6" r:id="rId5" xr:uid="{3032ED9C-BF7B-4835-B707-8EBF94637F00}"/>
-    <hyperlink ref="K7" r:id="rId6" xr:uid="{82419342-953D-4B49-93FF-7C924BB80AC1}"/>
+    <hyperlink ref="J4" r:id="rId4" xr:uid="{C84373C9-1565-4B62-96B2-218A347D68E8}"/>
+    <hyperlink ref="J6" r:id="rId5" xr:uid="{3032ED9C-BF7B-4835-B707-8EBF94637F00}"/>
+    <hyperlink ref="J7" r:id="rId6" xr:uid="{82419342-953D-4B49-93FF-7C924BB80AC1}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>